<commit_message>
Excel Write + Confirmation Flow
Excel katakchalarini yangilash funksiyasini amalga oshirish va uni harakatni tasdiqlash oqimiga integratsiya qilish bajarildi
</commit_message>
<xml_diff>
--- a/data/example.xlsx
+++ b/data/example.xlsx
@@ -401,7 +401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -422,8 +422,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="str">
+        <v>Yangi Ism</v>
       </c>
       <c r="B2" t="str">
         <v>Firdavs</v>
@@ -517,7 +517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -550,9 +550,6 @@
       <c r="D2">
         <v>1200</v>
       </c>
-      <c r="E2">
-        <f>C2*D2</f>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -567,9 +564,6 @@
       <c r="D3">
         <v>800</v>
       </c>
-      <c r="E3">
-        <f>C3*D3</f>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -584,9 +578,6 @@
       <c r="D4">
         <v>1200</v>
       </c>
-      <c r="E4">
-        <f>C4*D4</f>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -601,9 +592,6 @@
       <c r="D5">
         <v>800</v>
       </c>
-      <c r="E5">
-        <f>C5*D5</f>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -618,9 +606,6 @@
       <c r="D6">
         <v>1200</v>
       </c>
-      <c r="E6">
-        <f>C6*D6</f>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -635,9 +620,6 @@
       <c r="D7">
         <v>800</v>
       </c>
-      <c r="E7">
-        <f>C7*D7</f>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -651,9 +633,6 @@
       </c>
       <c r="D8" t="str">
         <v>Grand Total:</v>
-      </c>
-      <c r="E8">
-        <f>SUM(E2:E7)</f>
       </c>
     </row>
   </sheetData>
@@ -667,7 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -700,9 +679,6 @@
       <c r="D2">
         <v>10</v>
       </c>
-      <c r="E2">
-        <f>IF(C2&gt;D2,"OK","Low")</f>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -717,9 +693,6 @@
       <c r="D3">
         <v>10</v>
       </c>
-      <c r="E3">
-        <f>IF(C3&gt;D3,"OK","Low")</f>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -734,9 +707,6 @@
       <c r="D4">
         <v>5</v>
       </c>
-      <c r="E4">
-        <f>IF(C4&gt;D4,"OK","Low")</f>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -751,9 +721,6 @@
       <c r="D5">
         <v>20</v>
       </c>
-      <c r="E5">
-        <f>IF(C5&gt;D5,"OK","Low")</f>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -767,9 +734,6 @@
       </c>
       <c r="D6">
         <v>15</v>
-      </c>
-      <c r="E6">
-        <f>IF(C6&gt;D6,"OK","Low")</f>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Formula Explanation Tool uchun prompt tayyor
</commit_message>
<xml_diff>
--- a/data/example.xlsx
+++ b/data/example.xlsx
@@ -401,7 +401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -422,8 +422,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>Yangi Ism</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="str">
         <v>Firdavs</v>
@@ -517,7 +517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -550,6 +550,10 @@
       <c r="D2">
         <v>1200</v>
       </c>
+      <c r="E2">
+        <f>C2*D2</f>
+        <v>12000</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -564,6 +568,10 @@
       <c r="D3">
         <v>800</v>
       </c>
+      <c r="E3">
+        <f>C3*D3</f>
+        <v>20000</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -578,6 +586,10 @@
       <c r="D4">
         <v>1200</v>
       </c>
+      <c r="E4">
+        <f>C4*D4</f>
+        <v>18000</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -592,6 +604,10 @@
       <c r="D5">
         <v>800</v>
       </c>
+      <c r="E5">
+        <f>C5*D5</f>
+        <v>24000</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -606,6 +622,10 @@
       <c r="D6">
         <v>1200</v>
       </c>
+      <c r="E6">
+        <f>C6*D6</f>
+        <v>24000</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -620,6 +640,10 @@
       <c r="D7">
         <v>800</v>
       </c>
+      <c r="E7">
+        <f>C7*D7</f>
+        <v>32000</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -633,6 +657,10 @@
       </c>
       <c r="D8" t="str">
         <v>Grand Total:</v>
+      </c>
+      <c r="E8">
+        <f>SUM(E2:E7)</f>
+        <v>130000</v>
       </c>
     </row>
   </sheetData>
@@ -646,7 +674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -679,6 +707,10 @@
       <c r="D2">
         <v>10</v>
       </c>
+      <c r="E2" t="str">
+        <f>IF(C2&gt;D2,"OK","Low")</f>
+        <v>OK</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -693,6 +725,10 @@
       <c r="D3">
         <v>10</v>
       </c>
+      <c r="E3" t="str">
+        <f>IF(C3&gt;D3,"OK","Low")</f>
+        <v>Low</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -707,6 +743,10 @@
       <c r="D4">
         <v>5</v>
       </c>
+      <c r="E4" t="str">
+        <f>IF(C4&gt;D4,"OK","Low")</f>
+        <v>OK</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -721,6 +761,10 @@
       <c r="D5">
         <v>20</v>
       </c>
+      <c r="E5" t="str">
+        <f>IF(C5&gt;D5,"OK","Low")</f>
+        <v>OK</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -734,6 +778,10 @@
       </c>
       <c r="D6">
         <v>15</v>
+      </c>
+      <c r="E6" t="str">
+        <f>IF(C6&gt;D6,"OK","Low")</f>
+        <v>Low</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
open ai bilan integratsiya qo'shildi
</commit_message>
<xml_diff>
--- a/data/example.xlsx
+++ b/data/example.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -437,7 +437,7 @@
         <v>Engineering</v>
       </c>
       <c r="E2" s="1">
-        <v>5000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="3">
@@ -462,55 +462,21 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="str">
-        <v>Nodira</v>
+        <v>Lola</v>
       </c>
       <c r="C4" s="1" t="str">
-        <v>nodira@example.com</v>
+        <v>lola@gmail.com</v>
       </c>
       <c r="D4" s="1" t="str">
-        <v>HR</v>
+        <v>Hr</v>
       </c>
       <c r="E4" s="1">
-        <v>4800</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="str">
-        <v>Bekzod</v>
-      </c>
-      <c r="C5" s="1" t="str">
-        <v>bekzod@example.com</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <v>Engineering</v>
-      </c>
-      <c r="E5" s="1">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="str">
-        <v>Shaxriyor</v>
-      </c>
-      <c r="C6" s="1" t="str">
-        <v>shaxriyor@gmail.com</v>
-      </c>
-      <c r="D6" s="1" t="str">
-        <v>Developer</v>
-      </c>
-      <c r="E6" s="1">
-        <v>8000</v>
+        <v>4000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>